<commit_message>
updated automatic tab to fit screen size
</commit_message>
<xml_diff>
--- a/test_mixing_profiles.xlsx
+++ b/test_mixing_profiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/jonathanwulf_arizona_edu/Documents/College/ENGR 498 Senior Design/Code/T_Bioreactor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{F03370F3-CFAB-4F84-8BE0-CC3E4B6BADBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0337266E-C65D-4637-A1A1-144CC734B8B3}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{F03370F3-CFAB-4F84-8BE0-CC3E4B6BADBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A7431C6-CD1B-479B-8DF8-C70F3064BEF0}"/>
   <bookViews>
     <workbookView xWindow="3038" yWindow="3038" windowWidth="13680" windowHeight="9532" xr2:uid="{EEB3E656-C81F-49E1-B769-69393DB44D4C}"/>
   </bookViews>
@@ -409,7 +409,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -484,7 +484,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="B5">
         <v>75</v>

</xml_diff>

<commit_message>
updated profile for testing
</commit_message>
<xml_diff>
--- a/test_mixing_profiles.xlsx
+++ b/test_mixing_profiles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/jonathanwulf_arizona_edu/Documents/College/ENGR 498 Senior Design/Code/T_Bioreactor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{F03370F3-CFAB-4F84-8BE0-CC3E4B6BADBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{172B1952-BC95-417B-B7C4-6E97621CFE2A}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{F03370F3-CFAB-4F84-8BE0-CC3E4B6BADBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{039A2CD3-6A49-48F2-B2B0-D592FB794A93}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-2430" windowWidth="16440" windowHeight="28440" xr2:uid="{EEB3E656-C81F-49E1-B769-69393DB44D4C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EEB3E656-C81F-49E1-B769-69393DB44D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -103,10 +103,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -398,7 +394,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -408,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45E6529B-C724-4900-8C08-2B25F38260E9}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,10 +438,10 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -626,13 +622,13 @@
         <v>75</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>